<commit_message>
refined v1.2 of truncated screening report
</commit_message>
<xml_diff>
--- a/reports/Hit Summary.xlsx
+++ b/reports/Hit Summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve">Compound</t>
   </si>
@@ -29,56 +29,241 @@
     <t xml:space="preserve">MCULE-2500215977</t>
   </si>
   <si>
-    <t xml:space="preserve">quantile outlier hit</t>
+    <t xml:space="preserve">hit</t>
   </si>
   <si>
     <t xml:space="preserve">Tier 1</t>
   </si>
   <si>
+    <t xml:space="preserve">MCULE-1473251078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4886311520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6507164368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8738003894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4701897276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1862106206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9598397280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9383018269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5647507283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3983305475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6429987731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1287264115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2599558096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6664602135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7736239302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4137333334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4444789423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8098854428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8889584486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9409230926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8972325802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6585175330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1861200620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5535971573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5696626557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8006451741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7404167419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7072905523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7781963541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6708296378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7874963240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7049591067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9977367521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1167544378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6906295497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6595794580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3573602311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9671058458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2839632264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6745978470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4432971342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3233133913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9217060272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5098628920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1895483135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7859038199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7342632542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9216091708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7927011444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4648026737</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2241473973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9928629873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2424584680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2322746171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8229473821</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6724605060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1605214593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9200428087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5803429955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5026989357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9480521669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8963680177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3724067025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5051706074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3776534554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-3800615005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-7665114365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-9097980898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-6679712314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-5766769421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-1960141957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-8021080204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-2071926661</t>
+  </si>
+  <si>
     <t xml:space="preserve">MCULE-4074783148</t>
   </si>
   <si>
-    <t xml:space="preserve">MCULE-1473251078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-4886311520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-8738003894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-4701897276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-1862106206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-9383018269</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-5647507283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-3983305475</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-6429987731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-1287264115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-6507164368</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantile outlier hit,
-outlier %CV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCULE-9598397280</t>
+    <t xml:space="preserve">hit, tier 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCULE-4658147344</t>
   </si>
   <si>
     <t xml:space="preserve">MCULE-2233744168</t>
@@ -446,7 +631,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>2.3786540978763</v>
+        <v>2.42207069762061</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -460,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>2.42207069762061</v>
+        <v>2.65890902384315</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -474,7 +659,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>2.65890902384315</v>
+        <v>3.41374845693746</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -530,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>9.07226265405229</v>
+        <v>7.60200124952473</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -544,7 +729,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>18.3444007914478</v>
+        <v>9.07226265405229</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -558,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>19.2078226644461</v>
+        <v>18.3444007914478</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -572,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>21.9543922214425</v>
+        <v>19.2078226644461</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -586,7 +771,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>22.1922629409663</v>
+        <v>21.9543922214425</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -600,40 +785,782 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>3.41374845693746</v>
+        <v>22.1922629409663</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>18.5063381786124</v>
+        <v>17.8393941982523</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="n">
+        <v>18.8050121686289</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="n">
-        <v>30.113621563868</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B17" t="n">
+        <v>18.9599465350813</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20.536031925395</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="n">
+        <v>27.0891037890789</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>29.4804087587328</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="n">
+        <v>30.8806804382381</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="n">
+        <v>31.0841888222811</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="n">
+        <v>31.2445730309889</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="n">
+        <v>31.3965700043717</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="n">
+        <v>32.1002926778225</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="n">
+        <v>32.1813924356949</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="n">
+        <v>36.0462759640686</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="n">
+        <v>36.540781477331</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="n">
+        <v>37.0380485020154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="n">
+        <v>37.1492411565976</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="n">
+        <v>37.876832755798</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="n">
+        <v>38.0780098722503</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="n">
+        <v>39.1005766908364</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="n">
+        <v>41.2636844740255</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="n">
+        <v>41.6649498263898</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="n">
+        <v>45.1522292961625</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="n">
+        <v>45.4713103427483</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="n">
+        <v>45.8045182338763</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="n">
+        <v>45.8338637240896</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="n">
+        <v>45.8901996048702</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="n">
+        <v>45.9616182789438</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="n">
+        <v>49.7650860011356</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="n">
+        <v>52.4251892286287</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="n">
+        <v>53.3654256842655</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="n">
+        <v>53.5144976692846</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="n">
+        <v>53.5438095764513</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="n">
+        <v>53.8627287714998</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="n">
+        <v>54.7790970927613</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="n">
+        <v>55.3315833212513</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="n">
+        <v>55.5827497117479</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="n">
+        <v>55.6525919263283</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="n">
+        <v>56.3108536129857</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="n">
+        <v>57.0210392494812</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>57.9288708885863</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="n">
+        <v>58.5109216166103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="n">
+        <v>58.5728953631913</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="n">
+        <v>58.7663539504914</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="n">
+        <v>58.9945406070298</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="n">
+        <v>59.2986256590127</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="n">
+        <v>60.8653262638329</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>61.0355799129861</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>62.4186175834594</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="n">
+        <v>63.1849145851025</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" t="n">
+        <v>63.586068971755</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="n">
+        <v>63.7829221292224</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" t="n">
+        <v>64.4302697072097</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="n">
+        <v>64.5828599231672</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="n">
+        <v>64.6294514452372</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" t="n">
+        <v>65.127320251669</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" t="n">
+        <v>66.9308326423371</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" t="n">
+        <v>67.4849057051635</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="n">
+        <v>67.6816004231446</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>67.7759967304661</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="n">
+        <v>68.8898492027999</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" t="n">
+        <v>69.1712435116</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2.3786540978763</v>
+      </c>
+      <c r="C76" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" t="n">
+        <v>57.8731048230653</v>
+      </c>
+      <c r="C77" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" t="n">
+        <v>67.1191807086877</v>
+      </c>
+      <c r="C78"/>
+      <c r="D78" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>